<commit_message>
valid 0.8447, beta f1 0.8189
</commit_message>
<xml_diff>
--- a/实验数据.xlsx
+++ b/实验数据.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SunspotsRecognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6481311F-2020-4FF0-85E6-F5AE8F22F187}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269B7853-F571-44C2-8EB6-B181EDC9ACE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{FD2883F6-D81B-4C4E-8BFE-E8E8487B7D44}"/>
   </bookViews>
   <sheets>
-    <sheet name="continuum" sheetId="1" r:id="rId1"/>
+    <sheet name="数据集信息" sheetId="1" r:id="rId1"/>
     <sheet name="实验记录" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="49">
   <si>
     <t>alpha</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,10 +93,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>16-32-64-128-256</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Global Mean Pooling</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -119,10 +116,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>8-16-32-64-128</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Dataset</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -151,10 +144,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>32-64-128-256-512</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0004</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -190,34 +179,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Note</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>宽模型拟合能力更强</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mag比Con略差</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>同时使用两种数据有轻微提升</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>全局平均池化效果更好</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0006</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Momentum</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>beta F1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -234,7 +199,34 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Adam+SGD效果更好</t>
+    <t>1-8-16-32-64-128</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-16-32-64-128-256</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-16-32-64-128-256</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-32-64-128-256-512</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>Center Crop+Random Flip+Soft Voting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-16-32-64-128-256 * 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Image</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -245,7 +237,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0000_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,21 +298,27 @@
     </font>
     <font>
       <sz val="20"/>
-      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="20"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Var(--jp-code-font-family)"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +329,12 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -415,7 +419,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -458,6 +462,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -467,31 +486,33 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="176" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="15">
     <dxf>
-      <numFmt numFmtId="176" formatCode="0.0000_ "/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -503,9 +524,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="176" formatCode="0.0000_ "/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -574,23 +593,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3FEB377-C79F-4B70-B4A4-843E29A59236}" name="表1" displayName="表1" ref="A1:N21" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:N21" xr:uid="{C99BFBC0-C928-4177-AE40-416E97628F67}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{1CB02440-5C40-46B1-BD1F-9560F0337212}" name="ID" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{A52C51EB-FF62-4F99-ABD4-F7E9F742748B}" name="Dataset" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{8E0936CB-E80A-44BB-8A6C-0FB4F4243008}" name="Data Strategy" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{D5830E2B-78A3-4D53-B00C-7C767A38372F}" name="Model" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{222C7B3D-0812-48C9-8A3F-9C7DF753FB2F}" name="Architecture" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{C500A83B-70BD-41C8-8C03-965FC0BA7680}" name="Pooling" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{4C26B75D-30B8-4235-8F7B-15DBE3C26CC6}" name="Momentum" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{2735FE1C-7BA0-44DA-95B3-6066A9A0CFE8}" name="Optimizer" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{62233452-B367-4C74-8198-3227E6A540F6}" name="Train Acc" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{B88D0FE5-D709-462A-B4F7-56AB0EA59A11}" name="Valid Acc" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{0E917952-26A5-4EC8-AE9B-4D7675B68E5E}" name="beta F1" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{2168DAE4-2192-40F0-A6B8-794A6F04133C}" name="betax F1" dataDxfId="1"/>
-    <tableColumn id="17" xr3:uid="{E3FB10B3-700B-45E1-9AEF-6E445BD52EA2}" name="alpha F1" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{4E0FBDAF-83E0-40D2-A472-3F011AEB7ED9}" name="Note" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3FEB377-C79F-4B70-B4A4-843E29A59236}" name="表1" displayName="表1" ref="A1:M22" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:M22" xr:uid="{C99BFBC0-C928-4177-AE40-416E97628F67}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{1CB02440-5C40-46B1-BD1F-9560F0337212}" name="ID" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{A52C51EB-FF62-4F99-ABD4-F7E9F742748B}" name="Dataset" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{3A8EBDAE-10EA-4DD0-8D8B-310F4476573E}" name="Image" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{8E0936CB-E80A-44BB-8A6C-0FB4F4243008}" name="Data Strategy" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{D5830E2B-78A3-4D53-B00C-7C767A38372F}" name="Model" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{222C7B3D-0812-48C9-8A3F-9C7DF753FB2F}" name="Architecture" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{C500A83B-70BD-41C8-8C03-965FC0BA7680}" name="Pooling" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{2735FE1C-7BA0-44DA-95B3-6066A9A0CFE8}" name="Optimizer" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{62233452-B367-4C74-8198-3227E6A540F6}" name="Train Acc" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{B88D0FE5-D709-462A-B4F7-56AB0EA59A11}" name="Valid Acc" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{0E917952-26A5-4EC8-AE9B-4D7675B68E5E}" name="beta F1" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{2168DAE4-2192-40F0-A6B8-794A6F04133C}" name="betax F1" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{E3FB10B3-700B-45E1-9AEF-6E445BD52EA2}" name="alpha F1" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -896,10 +914,10 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="26.5546875" customWidth="1"/>
     <col min="2" max="2" width="20.109375" customWidth="1"/>
@@ -911,12 +929,12 @@
     <col min="9" max="9" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.8" thickBot="1">
       <c r="A1" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>3</v>
@@ -940,9 +958,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>23</v>
+    <row r="2" spans="1:9" ht="25.2">
+      <c r="A2" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>0</v>
@@ -970,8 +988,8 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+    <row r="3" spans="1:9" ht="25.2">
+      <c r="A3" s="20"/>
       <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
@@ -998,8 +1016,8 @@
         <v>733</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+    <row r="4" spans="1:9" ht="25.2">
+      <c r="A4" s="20"/>
       <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
@@ -1026,8 +1044,8 @@
         <v>763</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+    <row r="5" spans="1:9" ht="25.2">
+      <c r="A5" s="21"/>
       <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
@@ -1056,9 +1074,9 @@
         <v>763</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>33</v>
+    <row r="6" spans="1:9" ht="25.2">
+      <c r="A6" s="19" t="s">
+        <v>30</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>0</v>
@@ -1086,8 +1104,8 @@
         <v>730</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+    <row r="7" spans="1:9" ht="25.2">
+      <c r="A7" s="20"/>
       <c r="B7" s="12" t="s">
         <v>1</v>
       </c>
@@ -1114,8 +1132,8 @@
         <v>733</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+    <row r="8" spans="1:9" ht="25.2">
+      <c r="A8" s="20"/>
       <c r="B8" s="10" t="s">
         <v>2</v>
       </c>
@@ -1142,8 +1160,8 @@
         <v>763</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+    <row r="9" spans="1:9" ht="25.2">
+      <c r="A9" s="21"/>
       <c r="B9" s="12" t="s">
         <v>8</v>
       </c>
@@ -1185,96 +1203,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D91E81-82A9-4B1E-818E-A0189B8440F2}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="45.44140625" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.21875" customWidth="1"/>
-    <col min="5" max="5" width="37.33203125" customWidth="1"/>
-    <col min="6" max="6" width="38.21875" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" customWidth="1"/>
-    <col min="8" max="8" width="24.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="47.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.109375" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="46.6640625" customWidth="1"/>
+    <col min="7" max="7" width="38.21875" customWidth="1"/>
+    <col min="8" max="8" width="24.109375" customWidth="1"/>
     <col min="9" max="9" width="18.21875" customWidth="1"/>
     <col min="10" max="10" width="18.5546875" customWidth="1"/>
-    <col min="11" max="13" width="20.33203125" customWidth="1"/>
-    <col min="14" max="14" width="54.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
+    <col min="13" max="13" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="30" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2">
+        <v>224</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0.95</v>
+        <v>41</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I2" s="4">
         <v>0.89439999999999997</v>
@@ -1291,32 +1307,31 @@
       <c r="M2" s="4">
         <v>0.85429999999999995</v>
       </c>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" ht="30" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="C3" s="2">
+        <v>224</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0.98</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I3" s="4">
         <v>0.90910000000000002</v>
@@ -1333,245 +1348,255 @@
       <c r="M3" s="4">
         <v>0.85029999999999994</v>
       </c>
-      <c r="N3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1">
+      <c r="A4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="17">
+        <v>224</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="15">
+        <v>0.92530000000000001</v>
+      </c>
+      <c r="J4" s="15">
+        <v>0.79379999999999995</v>
+      </c>
+      <c r="K4" s="15">
+        <v>0.7581</v>
+      </c>
+      <c r="L4" s="15">
+        <v>0.75339999999999996</v>
+      </c>
+      <c r="M4" s="15">
+        <v>0.86219999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1">
+      <c r="A5" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="17">
+        <v>224</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="22">
+        <v>0.88280000000000003</v>
+      </c>
+      <c r="J5" s="22">
+        <v>0.77390000000000003</v>
+      </c>
+      <c r="K5" s="15">
+        <v>0.74709999999999999</v>
+      </c>
+      <c r="L5" s="15">
+        <v>0.76590000000000003</v>
+      </c>
+      <c r="M5" s="15">
+        <v>0.81499999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1">
+      <c r="A6" s="24"/>
+      <c r="B6" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="25">
+        <v>224</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27">
+        <v>0.84470000000000001</v>
+      </c>
+      <c r="K6" s="28">
+        <v>0.81889999999999996</v>
+      </c>
+      <c r="L6" s="28">
+        <v>0.83930000000000005</v>
+      </c>
+      <c r="M6" s="28">
+        <v>0.88109999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2">
+        <v>224</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="14">
+        <v>0.88429999999999997</v>
+      </c>
+      <c r="J7" s="14">
+        <v>0.78390000000000004</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0.74439999999999995</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.77129999999999999</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0.84040000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30" customHeight="1">
+      <c r="A8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2">
+        <v>224</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0.94350000000000001</v>
+      </c>
+      <c r="J8" s="14">
+        <v>0.76929999999999998</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="L8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="30" customHeight="1">
+      <c r="A9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="21" t="s">
+      <c r="C9" s="2">
+        <v>224</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="21">
-        <v>0.98</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="19">
-        <v>0.92530000000000001</v>
-      </c>
-      <c r="J4" s="19">
-        <v>0.79379999999999995</v>
-      </c>
-      <c r="K4" s="19">
-        <v>0.7581</v>
-      </c>
-      <c r="L4" s="19">
-        <v>0.75339999999999996</v>
-      </c>
-      <c r="M4" s="19">
-        <v>0.86219999999999997</v>
-      </c>
-      <c r="N4" s="21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="18">
-        <v>0.88280000000000003</v>
-      </c>
-      <c r="J5" s="18">
-        <v>0.77390000000000003</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0.74709999999999999</v>
-      </c>
-      <c r="L5" s="4">
-        <v>0.76590000000000003</v>
-      </c>
-      <c r="M5" s="4">
-        <v>0.81499999999999995</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="17">
-        <v>0.91300000000000003</v>
-      </c>
-      <c r="J6" s="17">
-        <v>0.79490000000000005</v>
-      </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="H9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="18">
-        <v>0.94350000000000001</v>
-      </c>
-      <c r="J7" s="18">
-        <v>0.76929999999999998</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="1:13" ht="30" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" ht="30" customHeight="1">
       <c r="A11" s="7"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1585,9 +1610,8 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:13" ht="30" customHeight="1">
       <c r="A12" s="7"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1601,9 +1625,8 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:13" ht="30" customHeight="1">
       <c r="A13" s="7"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1617,9 +1640,8 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:13" ht="30" customHeight="1">
       <c r="A14" s="7"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1633,9 +1655,8 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:13" ht="30" customHeight="1">
       <c r="A15" s="7"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1649,9 +1670,8 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:13" ht="30" customHeight="1">
       <c r="A16" s="7"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1665,9 +1685,8 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:13" ht="30" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1681,9 +1700,8 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:13" ht="30" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1697,9 +1715,8 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:13" ht="30" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1713,9 +1730,8 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:13" ht="30" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1729,9 +1745,8 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:13" ht="30" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1745,7 +1760,21 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
-      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" ht="30" customHeight="1">
+      <c r="A22" s="7"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1755,4 +1784,828 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79DD926-10CC-4129-B953-19FB4FC5D91D}">
+  <dimension ref="A1:B101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1">
+        <v>0.77490000000000003</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>0.77690000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>0.77739999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <v>0.77949999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>0.78049999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>0.78100000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <v>0.78249999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>0.78400000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9">
+        <v>0.78400000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10">
+        <v>0.78549999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>0.78710000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <v>0.78759999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>0.78859999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14">
+        <v>0.78910000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15">
+        <v>0.79059999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <v>0.79410000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17">
+        <v>0.79510000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18">
+        <v>0.79669999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19">
+        <v>0.79920000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20">
+        <v>0.79969999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21">
+        <v>0.80069999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22">
+        <v>0.80069999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23">
+        <v>0.80220000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24">
+        <v>0.80420000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25">
+        <v>0.80579999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26">
+        <v>0.80679999999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27">
+        <v>0.80779999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28">
+        <v>0.80879999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29">
+        <v>0.81340000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30">
+        <v>0.81440000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31">
+        <v>0.81340000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32">
+        <v>0.81489999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33">
+        <v>0.81540000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34">
+        <v>0.81840000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35">
+        <v>0.82199999999999995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36">
+        <v>0.82250000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <v>0.82350000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>0.82550000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39">
+        <v>0.82799999999999996</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40">
+        <v>0.83509999999999995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41">
+        <v>0.83609999999999995</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42">
+        <v>0.83809999999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43">
+        <v>0.83709999999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44">
+        <v>0.83809999999999996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <v>0.8407</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>0.84319999999999995</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>0.84219999999999995</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>0.84470000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49">
+        <v>0.84770000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50">
+        <v>0.8488</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51">
+        <v>0.84470000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52">
+        <v>0.84719999999999995</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53">
+        <v>0.8498</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B54">
+        <v>0.85129999999999995</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55">
+        <v>0.8508</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B56">
+        <v>0.84830000000000005</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57">
+        <v>0.84719999999999995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B58">
+        <v>0.84570000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59">
+        <v>0.84319999999999995</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60">
+        <v>0.84219999999999995</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B61">
+        <v>0.83709999999999996</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B62">
+        <v>0.83509999999999995</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B63">
+        <v>0.83409999999999995</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B64">
+        <v>0.8306</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B65">
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B66">
+        <v>0.82550000000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B67">
+        <v>0.82350000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68">
+        <v>0.82140000000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B69">
+        <v>0.81940000000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B70">
+        <v>0.81840000000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B71">
+        <v>0.81689999999999996</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B72">
+        <v>0.81589999999999996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B73">
+        <v>0.81440000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B74">
+        <v>0.81340000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B75">
+        <v>0.81279999999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B76">
+        <v>0.81279999999999997</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B77">
+        <v>0.81279999999999997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B78">
+        <v>0.81340000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B79">
+        <v>0.81130000000000002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B80">
+        <v>0.81130000000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B81">
+        <v>0.81130000000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B82">
+        <v>0.80979999999999996</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B83">
+        <v>0.80879999999999996</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B84">
+        <v>0.80979999999999996</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B85">
+        <v>0.80930000000000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B86">
+        <v>0.80879999999999996</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B87">
+        <v>0.81030000000000002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B88">
+        <v>0.81030000000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B89">
+        <v>0.80930000000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B90">
+        <v>0.80879999999999996</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B91">
+        <v>0.80779999999999996</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B92">
+        <v>0.80730000000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B93">
+        <v>0.80479999999999996</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B94">
+        <v>0.80269999999999997</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B95">
+        <v>0.80220000000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B96">
+        <v>0.80269999999999997</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B97">
+        <v>0.80220000000000002</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B98">
+        <v>0.80069999999999997</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B99">
+        <v>0.79920000000000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B100">
+        <v>0.79869999999999997</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B101">
+        <v>0.79820000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
valid acc 0.8604, beta f1 0.8328
</commit_message>
<xml_diff>
--- a/实验数据.xlsx
+++ b/实验数据.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SunspotsRecognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74706EDB-F4D4-481C-839B-579C42B5EB98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7354963-3462-4693-B1E4-DA2E30E9874C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{FD2883F6-D81B-4C4E-8BFE-E8E8487B7D44}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="85">
   <si>
     <t>alpha</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -184,18 +184,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>beta F1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>betax F1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>alpha F1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -219,10 +207,6 @@
     <t>accuracy</t>
   </si>
   <si>
-    <t>Center Crop+Random Flip+Soft Voting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1-16-32-64-128-256 * 2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -260,14 +244,130 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ccuracy</t>
-  </si>
-  <si>
     <t>0009</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Center Crop+Random Flip+Preprocess</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>过采样会降低beta F1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预处理不能提升准确率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加网络深度无效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全局最大池化不行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据融合效果不好</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加宽度轻微提升</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SGD效果好</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>概率层融合的效果更好</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DPN、ResNeXt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResNet14 * 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>双通道比数据融合效果好</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-16-32-64-128-256 * 2+256fc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加全连接无效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用320*320的图像、旋转数据增强</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Center Crop+Random Flip+Random Rot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机旋转无效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Center Crop+Random Flip+Zoom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zoom轻微提升</t>
+  </si>
+  <si>
+    <t>Zoom轻微提升</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13+3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Soft Voting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beta F1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Betax F1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alpha F1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0014</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -477,7 +577,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -556,6 +656,15 @@
     <xf numFmtId="176" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -565,17 +674,27 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0.0000_ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="176" formatCode="0.0000_ "/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -657,22 +776,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3FEB377-C79F-4B70-B4A4-843E29A59236}" name="表1" displayName="表1" ref="A1:M22" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:M22" xr:uid="{C99BFBC0-C928-4177-AE40-416E97628F67}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{1CB02440-5C40-46B1-BD1F-9560F0337212}" name="ID" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{A52C51EB-FF62-4F99-ABD4-F7E9F742748B}" name="Dataset" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{3A8EBDAE-10EA-4DD0-8D8B-310F4476573E}" name="Image" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{8E0936CB-E80A-44BB-8A6C-0FB4F4243008}" name="Data Strategy" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{D5830E2B-78A3-4D53-B00C-7C767A38372F}" name="Model" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{222C7B3D-0812-48C9-8A3F-9C7DF753FB2F}" name="Architecture" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{C500A83B-70BD-41C8-8C03-965FC0BA7680}" name="Pooling" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{2735FE1C-7BA0-44DA-95B3-6066A9A0CFE8}" name="Optimizer" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{62233452-B367-4C74-8198-3227E6A540F6}" name="Train Acc" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{B88D0FE5-D709-462A-B4F7-56AB0EA59A11}" name="Valid Acc" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{0E917952-26A5-4EC8-AE9B-4D7675B68E5E}" name="beta F1" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{2168DAE4-2192-40F0-A6B8-794A6F04133C}" name="betax F1" dataDxfId="1"/>
-    <tableColumn id="17" xr3:uid="{E3FB10B3-700B-45E1-9AEF-6E445BD52EA2}" name="alpha F1" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3FEB377-C79F-4B70-B4A4-843E29A59236}" name="表1" displayName="表1" ref="A1:N23" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:N23" xr:uid="{C99BFBC0-C928-4177-AE40-416E97628F67}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N23">
+    <sortCondition ref="A1:A23"/>
+  </sortState>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{1CB02440-5C40-46B1-BD1F-9560F0337212}" name="ID" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{A52C51EB-FF62-4F99-ABD4-F7E9F742748B}" name="Dataset" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{3A8EBDAE-10EA-4DD0-8D8B-310F4476573E}" name="Image" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{8E0936CB-E80A-44BB-8A6C-0FB4F4243008}" name="Data Strategy" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{D5830E2B-78A3-4D53-B00C-7C767A38372F}" name="Model" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{222C7B3D-0812-48C9-8A3F-9C7DF753FB2F}" name="Architecture" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{C500A83B-70BD-41C8-8C03-965FC0BA7680}" name="Pooling" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{2735FE1C-7BA0-44DA-95B3-6066A9A0CFE8}" name="Optimizer" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{62233452-B367-4C74-8198-3227E6A540F6}" name="Train Acc" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{B88D0FE5-D709-462A-B4F7-56AB0EA59A11}" name="Valid Acc" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{0E917952-26A5-4EC8-AE9B-4D7675B68E5E}" name="Beta F1" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{2168DAE4-2192-40F0-A6B8-794A6F04133C}" name="Betax F1" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{E3FB10B3-700B-45E1-9AEF-6E445BD52EA2}" name="Alpha F1" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{BD065C81-EC90-4450-9E6A-7714E5147B0D}" name="Note" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1023,7 +1146,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="25.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -1053,7 +1176,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="25.2">
-      <c r="A3" s="27"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
@@ -1081,7 +1204,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="25.2">
-      <c r="A4" s="27"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
@@ -1109,7 +1232,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="25.2">
-      <c r="A5" s="28"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
@@ -1139,7 +1262,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="25.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="29" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1169,7 +1292,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="25.2">
-      <c r="A7" s="27"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="12" t="s">
         <v>1</v>
       </c>
@@ -1197,7 +1320,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="25.2">
-      <c r="A8" s="27"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="10" t="s">
         <v>2</v>
       </c>
@@ -1225,7 +1348,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="25.2">
-      <c r="A9" s="28"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="12" t="s">
         <v>8</v>
       </c>
@@ -1267,10 +1390,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D91E81-82A9-4B1E-818E-A0189B8440F2}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1278,9 +1401,9 @@
     <col min="1" max="1" width="11.5546875" customWidth="1"/>
     <col min="2" max="2" width="47.5546875" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="68.5546875" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" customWidth="1"/>
-    <col min="6" max="6" width="46.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.109375" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="53.109375" customWidth="1"/>
     <col min="7" max="7" width="38.21875" customWidth="1"/>
     <col min="8" max="8" width="24.109375" customWidth="1"/>
     <col min="9" max="9" width="18.21875" customWidth="1"/>
@@ -1288,9 +1411,10 @@
     <col min="11" max="11" width="18.44140625" customWidth="1"/>
     <col min="12" max="12" width="19" customWidth="1"/>
     <col min="13" max="13" width="20.44140625" customWidth="1"/>
+    <col min="14" max="14" width="42.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1">
+    <row r="1" spans="1:14" ht="30" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -1298,7 +1422,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>18</v>
@@ -1322,16 +1446,19 @@
         <v>16</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1">
+        <v>83</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
@@ -1348,7 +1475,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>14</v>
@@ -1371,8 +1498,9 @@
       <c r="M2" s="4">
         <v>0.85429999999999995</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="30" customHeight="1">
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:14" s="26" customFormat="1" ht="30" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>24</v>
       </c>
@@ -1389,72 +1517,78 @@
         <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0.92530000000000001</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.79379999999999995</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0.7581</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0.75339999999999996</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0.86219999999999997</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2">
+        <v>224</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I4" s="4">
         <v>0.90910000000000002</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J4" s="4">
         <v>0.78400000000000003</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K4" s="4">
         <v>0.75070000000000003</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L4" s="4">
         <v>0.74460000000000004</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M4" s="4">
         <v>0.85029999999999994</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="17">
-        <v>224</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="15">
-        <v>0.92530000000000001</v>
-      </c>
-      <c r="J4" s="15">
-        <v>0.79379999999999995</v>
-      </c>
-      <c r="K4" s="15">
-        <v>0.7581</v>
-      </c>
-      <c r="L4" s="15">
-        <v>0.75339999999999996</v>
-      </c>
-      <c r="M4" s="15">
-        <v>0.86219999999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1">
+      <c r="N4" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>25</v>
       </c>
@@ -1471,7 +1605,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>14</v>
@@ -1494,51 +1628,55 @@
       <c r="M5" s="15">
         <v>0.81499999999999995</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="22" t="s">
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="2">
         <v>224</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="23" t="s">
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="23" t="s">
+      <c r="F6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="24">
-        <v>0.96519999999999995</v>
-      </c>
-      <c r="J6" s="24">
-        <v>0.84470000000000001</v>
-      </c>
-      <c r="K6" s="25">
-        <v>0.81889999999999996</v>
-      </c>
-      <c r="L6" s="25">
-        <v>0.83930000000000005</v>
-      </c>
-      <c r="M6" s="25">
-        <v>0.88109999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1">
+      <c r="I6" s="14">
+        <v>0.88429999999999997</v>
+      </c>
+      <c r="J6" s="14">
+        <v>0.78390000000000004</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0.74439999999999995</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0.77129999999999999</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0.84040000000000004</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>26</v>
@@ -1553,130 +1691,139 @@
         <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>34</v>
       </c>
       <c r="I7" s="14">
-        <v>0.88429999999999997</v>
+        <v>0.94350000000000001</v>
       </c>
       <c r="J7" s="14">
-        <v>0.78390000000000004</v>
-      </c>
-      <c r="K7" s="4">
-        <v>0.74439999999999995</v>
-      </c>
-      <c r="L7" s="4">
-        <v>0.77129999999999999</v>
-      </c>
-      <c r="M7" s="4">
-        <v>0.84040000000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="30" customHeight="1">
-      <c r="A8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="2" t="s">
+        <v>0.76929999999999998</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
+      <c r="A8" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="17">
         <v>224</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="F8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="14">
-        <v>0.94350000000000001</v>
-      </c>
-      <c r="J8" s="14">
-        <v>0.76929999999999998</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="18" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="17" t="s">
+      <c r="I8" s="19">
+        <v>0.94579999999999997</v>
+      </c>
+      <c r="J8" s="19">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="K8" s="19">
+        <v>0.76590000000000003</v>
+      </c>
+      <c r="L8" s="19">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="M8" s="19">
+        <v>0.8619</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
+      <c r="A9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="2">
         <v>224</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="17" t="s">
+      <c r="E9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="19">
-        <v>0.94579999999999997</v>
-      </c>
-      <c r="J9" s="19">
-        <v>0.80200000000000005</v>
-      </c>
-      <c r="K9" s="19">
-        <v>0.76590000000000003</v>
-      </c>
-      <c r="L9" s="19">
-        <v>0.77800000000000002</v>
-      </c>
-      <c r="M9" s="19">
-        <v>0.8619</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="30" customHeight="1">
+      <c r="I9" s="4">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0.75880000000000003</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0.78359999999999996</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0.86850000000000005</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2">
         <v>224</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>14</v>
@@ -1685,24 +1832,27 @@
         <v>34</v>
       </c>
       <c r="I10" s="4">
-        <v>0.84730000000000005</v>
+        <v>0.92410000000000003</v>
       </c>
       <c r="J10" s="4">
-        <v>0.80300000000000005</v>
+        <v>0.80349999999999999</v>
       </c>
       <c r="K10" s="4">
-        <v>0.75880000000000003</v>
-      </c>
-      <c r="L10" s="4">
-        <v>0.78359999999999996</v>
-      </c>
-      <c r="M10" s="4">
-        <v>0.86850000000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="29" customFormat="1" ht="30" customHeight="1">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="L10" s="27">
+        <v>0.79890000000000005</v>
+      </c>
+      <c r="M10" s="27">
+        <v>0.87380000000000002</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="26" customFormat="1" ht="30" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>21</v>
@@ -1711,13 +1861,13 @@
         <v>224</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>14</v>
@@ -1726,39 +1876,42 @@
         <v>34</v>
       </c>
       <c r="I11" s="4">
-        <v>0.92410000000000003</v>
+        <v>0.94850000000000001</v>
       </c>
       <c r="J11" s="4">
-        <v>0.80349999999999999</v>
+        <v>0.77039999999999997</v>
       </c>
       <c r="K11" s="4">
-        <v>0.73699999999999999</v>
-      </c>
-      <c r="L11" s="30">
-        <v>0.79890000000000005</v>
-      </c>
-      <c r="M11" s="30">
-        <v>0.87380000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1">
+        <v>0.73070000000000002</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0.74380000000000002</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0.83840000000000003</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2">
         <v>224</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>14</v>
@@ -1767,112 +1920,277 @@
         <v>34</v>
       </c>
       <c r="I12" s="4">
-        <v>0.94850000000000001</v>
+        <v>0.92720000000000002</v>
       </c>
       <c r="J12" s="4">
-        <v>0.77039999999999997</v>
+        <v>0.81340000000000001</v>
       </c>
       <c r="K12" s="4">
-        <v>0.73070000000000002</v>
+        <v>0.78149999999999997</v>
       </c>
       <c r="L12" s="4">
-        <v>0.74380000000000002</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="M12" s="4">
-        <v>0.83840000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="30" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-    </row>
-    <row r="14" spans="1:13" ht="30" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-    </row>
-    <row r="15" spans="1:13" ht="30" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-    </row>
-    <row r="16" spans="1:13" ht="30" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-    </row>
-    <row r="17" spans="1:13" ht="30" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-    </row>
-    <row r="18" spans="1:13" ht="30" customHeight="1">
-      <c r="A18" s="7"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-    </row>
-    <row r="19" spans="1:13" ht="30" customHeight="1">
+        <v>0.85860000000000003</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30" customHeight="1">
+      <c r="A13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2">
+        <v>224</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0.80779999999999996</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0.77749999999999997</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0.84909999999999997</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="30" customHeight="1">
+      <c r="A14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="2">
+        <v>224</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0.88039999999999996</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0.79559999999999997</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0.75290000000000001</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0.74450000000000005</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0.87770000000000004</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30" customHeight="1">
+      <c r="A15" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="17">
+        <v>224</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="15">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="J15" s="15">
+        <v>0.81289999999999996</v>
+      </c>
+      <c r="K15" s="15">
+        <v>0.76880000000000004</v>
+      </c>
+      <c r="L15" s="15">
+        <v>0.79979999999999996</v>
+      </c>
+      <c r="M15" s="15">
+        <v>0.87070000000000003</v>
+      </c>
+      <c r="N15" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="26" customFormat="1" ht="30" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="2">
+        <v>320</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="22">
+        <v>224</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="24">
+        <v>0.96609999999999996</v>
+      </c>
+      <c r="J17" s="24">
+        <v>0.86040000000000005</v>
+      </c>
+      <c r="K17" s="25">
+        <v>0.83279999999999998</v>
+      </c>
+      <c r="L17" s="25">
+        <v>0.85829999999999995</v>
+      </c>
+      <c r="M17" s="25">
+        <v>0.89549999999999996</v>
+      </c>
+      <c r="N17" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="26" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="33">
+        <v>224</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="35">
+        <v>0.96519999999999995</v>
+      </c>
+      <c r="J18" s="35">
+        <v>0.84470000000000001</v>
+      </c>
+      <c r="K18" s="28">
+        <v>0.81889999999999996</v>
+      </c>
+      <c r="L18" s="28">
+        <v>0.83930000000000005</v>
+      </c>
+      <c r="M18" s="28">
+        <v>0.88109999999999999</v>
+      </c>
+      <c r="N18" s="28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="30" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1886,8 +2204,9 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-    </row>
-    <row r="20" spans="1:13" ht="30" customHeight="1">
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="1:14" ht="30" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1901,8 +2220,9 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
-    </row>
-    <row r="21" spans="1:13" ht="30" customHeight="1">
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="1:14" ht="30" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1916,12 +2236,15 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
-    </row>
-    <row r="22" spans="1:13" ht="30" customHeight="1">
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" ht="30" customHeight="1">
       <c r="A22" s="7"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="D22" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1931,6 +2254,25 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" ht="30" customHeight="1">
+      <c r="A23" s="7"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1954,7 +2296,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1">
         <v>0.77490000000000003</v>
@@ -1962,7 +2304,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>0.77690000000000003</v>
@@ -1970,7 +2312,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>0.77739999999999998</v>
@@ -1978,7 +2320,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>0.77949999999999997</v>
@@ -1986,7 +2328,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>0.78049999999999997</v>
@@ -1994,7 +2336,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>0.78100000000000003</v>
@@ -2002,7 +2344,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>0.78249999999999997</v>
@@ -2010,7 +2352,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>0.78400000000000003</v>
@@ -2018,7 +2360,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9">
         <v>0.78400000000000003</v>
@@ -2026,7 +2368,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>0.78549999999999998</v>
@@ -2034,7 +2376,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B11">
         <v>0.78710000000000002</v>
@@ -2042,7 +2384,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>0.78759999999999997</v>
@@ -2050,7 +2392,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <v>0.78859999999999997</v>
@@ -2058,7 +2400,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14">
         <v>0.78910000000000002</v>
@@ -2066,7 +2408,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>0.79059999999999997</v>
@@ -2074,7 +2416,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>0.79410000000000003</v>
@@ -2082,7 +2424,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>0.79510000000000003</v>
@@ -2090,7 +2432,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <v>0.79669999999999996</v>
@@ -2098,7 +2440,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B19">
         <v>0.79920000000000002</v>
@@ -2106,7 +2448,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B20">
         <v>0.79969999999999997</v>
@@ -2114,7 +2456,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B21">
         <v>0.80069999999999997</v>
@@ -2122,7 +2464,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B22">
         <v>0.80069999999999997</v>
@@ -2130,7 +2472,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B23">
         <v>0.80220000000000002</v>
@@ -2138,7 +2480,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B24">
         <v>0.80420000000000003</v>
@@ -2146,7 +2488,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B25">
         <v>0.80579999999999996</v>
@@ -2154,7 +2496,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B26">
         <v>0.80679999999999996</v>
@@ -2162,7 +2504,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B27">
         <v>0.80779999999999996</v>
@@ -2170,7 +2512,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B28">
         <v>0.80879999999999996</v>
@@ -2178,7 +2520,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B29">
         <v>0.81340000000000001</v>
@@ -2186,7 +2528,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B30">
         <v>0.81440000000000001</v>
@@ -2194,7 +2536,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B31">
         <v>0.81340000000000001</v>
@@ -2202,7 +2544,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B32">
         <v>0.81489999999999996</v>
@@ -2210,7 +2552,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B33">
         <v>0.81540000000000001</v>
@@ -2218,7 +2560,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B34">
         <v>0.81840000000000002</v>
@@ -2226,7 +2568,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B35">
         <v>0.82199999999999995</v>
@@ -2234,7 +2576,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B36">
         <v>0.82250000000000001</v>
@@ -2242,7 +2584,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B37">
         <v>0.82350000000000001</v>
@@ -2250,7 +2592,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B38">
         <v>0.82550000000000001</v>
@@ -2258,7 +2600,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B39">
         <v>0.82799999999999996</v>
@@ -2266,7 +2608,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B40">
         <v>0.83509999999999995</v>
@@ -2274,7 +2616,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>0.83609999999999995</v>
@@ -2282,7 +2624,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B42">
         <v>0.83809999999999996</v>
@@ -2290,7 +2632,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B43">
         <v>0.83709999999999996</v>
@@ -2298,7 +2640,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>0.83809999999999996</v>
@@ -2306,7 +2648,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B45">
         <v>0.8407</v>
@@ -2314,7 +2656,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B46">
         <v>0.84319999999999995</v>
@@ -2322,7 +2664,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B47">
         <v>0.84219999999999995</v>
@@ -2330,7 +2672,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B48">
         <v>0.84470000000000001</v>
@@ -2338,7 +2680,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B49">
         <v>0.84770000000000001</v>
@@ -2346,7 +2688,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B50">
         <v>0.8488</v>
@@ -2354,7 +2696,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B51">
         <v>0.84470000000000001</v>
@@ -2362,7 +2704,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B52">
         <v>0.84719999999999995</v>
@@ -2370,7 +2712,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B53">
         <v>0.8498</v>
@@ -2378,7 +2720,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B54">
         <v>0.85129999999999995</v>
@@ -2386,7 +2728,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B55">
         <v>0.8508</v>
@@ -2394,7 +2736,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B56">
         <v>0.84830000000000005</v>
@@ -2402,7 +2744,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B57">
         <v>0.84719999999999995</v>
@@ -2410,7 +2752,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B58">
         <v>0.84570000000000001</v>
@@ -2418,7 +2760,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B59">
         <v>0.84319999999999995</v>
@@ -2426,7 +2768,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B60">
         <v>0.84219999999999995</v>
@@ -2434,7 +2776,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B61">
         <v>0.83709999999999996</v>
@@ -2442,7 +2784,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B62">
         <v>0.83509999999999995</v>
@@ -2450,7 +2792,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B63">
         <v>0.83409999999999995</v>
@@ -2458,7 +2800,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B64">
         <v>0.8306</v>
@@ -2466,7 +2808,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B65">
         <v>0.82499999999999996</v>
@@ -2474,7 +2816,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B66">
         <v>0.82550000000000001</v>
@@ -2482,7 +2824,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B67">
         <v>0.82350000000000001</v>
@@ -2490,7 +2832,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B68">
         <v>0.82140000000000002</v>
@@ -2498,7 +2840,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B69">
         <v>0.81940000000000002</v>
@@ -2506,7 +2848,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B70">
         <v>0.81840000000000002</v>
@@ -2514,7 +2856,7 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B71">
         <v>0.81689999999999996</v>
@@ -2522,7 +2864,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B72">
         <v>0.81589999999999996</v>
@@ -2530,7 +2872,7 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B73">
         <v>0.81440000000000001</v>
@@ -2538,7 +2880,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B74">
         <v>0.81340000000000001</v>
@@ -2546,7 +2888,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B75">
         <v>0.81279999999999997</v>
@@ -2554,7 +2896,7 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B76">
         <v>0.81279999999999997</v>
@@ -2562,7 +2904,7 @@
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B77">
         <v>0.81279999999999997</v>
@@ -2570,7 +2912,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B78">
         <v>0.81340000000000001</v>
@@ -2578,7 +2920,7 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B79">
         <v>0.81130000000000002</v>
@@ -2586,7 +2928,7 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B80">
         <v>0.81130000000000002</v>
@@ -2594,7 +2936,7 @@
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B81">
         <v>0.81130000000000002</v>
@@ -2602,7 +2944,7 @@
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B82">
         <v>0.80979999999999996</v>
@@ -2610,7 +2952,7 @@
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B83">
         <v>0.80879999999999996</v>
@@ -2618,7 +2960,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B84">
         <v>0.80979999999999996</v>
@@ -2626,7 +2968,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B85">
         <v>0.80930000000000002</v>
@@ -2634,7 +2976,7 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B86">
         <v>0.80879999999999996</v>
@@ -2642,7 +2984,7 @@
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B87">
         <v>0.81030000000000002</v>
@@ -2650,7 +2992,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B88">
         <v>0.81030000000000002</v>
@@ -2658,7 +3000,7 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B89">
         <v>0.80930000000000002</v>
@@ -2666,7 +3008,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B90">
         <v>0.80879999999999996</v>
@@ -2674,7 +3016,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B91">
         <v>0.80779999999999996</v>
@@ -2682,7 +3024,7 @@
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B92">
         <v>0.80730000000000002</v>
@@ -2690,7 +3032,7 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B93">
         <v>0.80479999999999996</v>
@@ -2698,7 +3040,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B94">
         <v>0.80269999999999997</v>
@@ -2706,7 +3048,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B95">
         <v>0.80220000000000002</v>
@@ -2714,7 +3056,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B96">
         <v>0.80269999999999997</v>
@@ -2722,7 +3064,7 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B97">
         <v>0.80220000000000002</v>
@@ -2730,7 +3072,7 @@
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B98">
         <v>0.80069999999999997</v>
@@ -2738,7 +3080,7 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B99">
         <v>0.79920000000000002</v>
@@ -2746,7 +3088,7 @@
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B100">
         <v>0.79869999999999997</v>
@@ -2754,7 +3096,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B101">
         <v>0.79820000000000002</v>
@@ -2769,112 +3111,209 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FEA663-630A-4D72-8252-EC0CC7D44DAA}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B1">
-        <v>0.80269999999999997</v>
+        <v>0.80020000000000002</v>
       </c>
       <c r="C1">
-        <f>B1+B6</f>
-        <v>1.6069</v>
+        <f>B1+B6+B11+B16+B21</f>
+        <v>4.0647000000000002</v>
       </c>
       <c r="D1">
-        <f>C1/2</f>
-        <v>0.80345</v>
+        <f>C1/5</f>
+        <v>0.81294</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B2">
-        <v>0.7369</v>
+        <v>0.76249999999999996</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C4" si="0">B2+B7</f>
-        <v>1.4739</v>
+        <f t="shared" ref="C2:C4" si="0">B2+B7+B12+B17+B22</f>
+        <v>3.8441999999999998</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D4" si="1">C2/2</f>
-        <v>0.73694999999999999</v>
+        <f t="shared" ref="D2:D4" si="1">C2/5</f>
+        <v>0.76883999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B3">
-        <v>0.79769999999999996</v>
+        <v>0.76519999999999999</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
-        <v>1.5977000000000001</v>
+        <v>3.9990999999999999</v>
       </c>
       <c r="D3">
         <f t="shared" si="1"/>
-        <v>0.79885000000000006</v>
+        <v>0.79981999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B4">
-        <v>0.87290000000000001</v>
+        <v>0.86619999999999997</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>1.7475000000000001</v>
+        <v>4.3533999999999997</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>0.87375000000000003</v>
+        <v>0.8706799999999999</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B6">
-        <v>0.80420000000000003</v>
+        <v>0.81079999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B7">
-        <v>0.73699999999999999</v>
+        <v>0.76429999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B8">
-        <v>0.8</v>
+        <v>0.80210000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B9">
+        <v>0.86939999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11">
+        <v>0.80420000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <v>0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <v>0.86439999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
+        <v>0.82750000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17">
+        <v>0.78139999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18">
+        <v>0.82520000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19">
+        <v>0.87880000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21">
+        <v>0.82199999999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23">
+        <v>0.8266</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24">
         <v>0.87460000000000004</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
valid acc 0.8837, beta f1 0.8606
</commit_message>
<xml_diff>
--- a/实验数据.xlsx
+++ b/实验数据.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SunspotsRecognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7354963-3462-4693-B1E4-DA2E30E9874C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFB876B-0271-4BB2-98AA-21BC58E62F79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{FD2883F6-D81B-4C4E-8BFE-E8E8487B7D44}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="93">
   <si>
     <t>alpha</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,10 +94,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Global Mean Pooling</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Pooling</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -288,10 +284,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>概率层融合的效果更好</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DPN、ResNeXt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -316,10 +308,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>使用320*320的图像、旋转数据增强</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0012</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -368,6 +356,49 @@
   </si>
   <si>
     <t>0014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>概率融合效果好</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>320轻微提升</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14+15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>320+Zoom轻微提升</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>320+Zoom提升4个点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Global Average Pooling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResNeXt14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>ResNeXt14轻微提升</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -378,7 +409,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0000_ "/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,14 +476,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="20"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Var(--jp-code-font-family)"/>
@@ -467,9 +490,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="20"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="20"/>
-      <color theme="4" tint="-0.499984740745262"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -635,36 +675,27 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -674,17 +705,26 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -776,10 +816,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3FEB377-C79F-4B70-B4A4-843E29A59236}" name="表1" displayName="表1" ref="A1:N23" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:N23" xr:uid="{C99BFBC0-C928-4177-AE40-416E97628F67}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N23">
-    <sortCondition ref="A1:A23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3FEB377-C79F-4B70-B4A4-843E29A59236}" name="表1" displayName="表1" ref="A1:N26" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:N26" xr:uid="{C99BFBC0-C928-4177-AE40-416E97628F67}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N26">
+    <sortCondition ref="A1:A26"/>
   </sortState>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{1CB02440-5C40-46B1-BD1F-9560F0337212}" name="ID" dataDxfId="13"/>
@@ -1118,10 +1158,10 @@
   <sheetData>
     <row r="1" spans="1:9" ht="25.8" thickBot="1">
       <c r="A1" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>3</v>
@@ -1146,8 +1186,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="25.2">
-      <c r="A2" s="29" t="s">
-        <v>21</v>
+      <c r="A2" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>0</v>
@@ -1176,7 +1216,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="25.2">
-      <c r="A3" s="30"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
@@ -1204,7 +1244,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="25.2">
-      <c r="A4" s="30"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
@@ -1232,7 +1272,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="25.2">
-      <c r="A5" s="31"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
@@ -1262,8 +1302,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="25.2">
-      <c r="A6" s="29" t="s">
-        <v>30</v>
+      <c r="A6" s="26" t="s">
+        <v>29</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>0</v>
@@ -1292,7 +1332,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="25.2">
-      <c r="A7" s="30"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="12" t="s">
         <v>1</v>
       </c>
@@ -1320,7 +1360,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="25.2">
-      <c r="A8" s="30"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="10" t="s">
         <v>2</v>
       </c>
@@ -1348,7 +1388,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="25.2">
-      <c r="A9" s="31"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="12" t="s">
         <v>8</v>
       </c>
@@ -1390,21 +1430,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D91E81-82A9-4B1E-818E-A0189B8440F2}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
     <col min="2" max="2" width="47.5546875" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="67.109375" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" customWidth="1"/>
     <col min="6" max="6" width="53.109375" customWidth="1"/>
-    <col min="7" max="7" width="38.21875" customWidth="1"/>
+    <col min="7" max="7" width="42" customWidth="1"/>
     <col min="8" max="8" width="24.109375" customWidth="1"/>
     <col min="9" max="9" width="18.21875" customWidth="1"/>
     <col min="10" max="10" width="18.5546875" customWidth="1"/>
@@ -1416,16 +1456,16 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>12</v>
@@ -1434,54 +1474,54 @@
         <v>13</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2">
         <v>224</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" s="4">
         <v>0.89439999999999997</v>
@@ -1500,30 +1540,30 @@
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" s="26" customFormat="1" ht="30" customHeight="1">
+    <row r="3" spans="1:14" s="20" customFormat="1" ht="30" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2">
         <v>224</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="4">
         <v>0.92530000000000001</v>
@@ -1541,33 +1581,33 @@
         <v>0.86219999999999997</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2">
         <v>224</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" s="4">
         <v>0.90910000000000002</v>
@@ -1585,75 +1625,75 @@
         <v>0.85029999999999994</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="17">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="20" customFormat="1" ht="30" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2">
         <v>224</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="17" t="s">
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="19">
+      <c r="F5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="14">
         <v>0.88280000000000003</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="14">
         <v>0.77390000000000003</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="4">
         <v>0.74709999999999999</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="4">
         <v>0.76590000000000003</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="4">
         <v>0.81499999999999995</v>
       </c>
       <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2">
         <v>224</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="14">
         <v>0.88429999999999997</v>
@@ -1671,33 +1711,33 @@
         <v>0.84040000000000004</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2">
         <v>224</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" s="14">
         <v>0.94350000000000001</v>
@@ -1706,86 +1746,86 @@
         <v>0.76929999999999998</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="17">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="20" customFormat="1" ht="30" customHeight="1">
+      <c r="A8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2">
         <v>224</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="17" t="s">
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="19">
+      <c r="F8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="14">
         <v>0.94579999999999997</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="14">
         <v>0.80200000000000005</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="14">
         <v>0.76590000000000003</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="14">
         <v>0.77800000000000002</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="14">
         <v>0.8619</v>
       </c>
-      <c r="N8" s="19" t="s">
-        <v>61</v>
+      <c r="N8" s="14" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2">
         <v>224</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I9" s="4">
         <v>0.84730000000000005</v>
@@ -1803,33 +1843,33 @@
         <v>0.86850000000000005</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="30" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="20" customFormat="1" ht="30" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2">
         <v>224</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="4">
         <v>0.92410000000000003</v>
@@ -1840,40 +1880,40 @@
       <c r="K10" s="4">
         <v>0.73699999999999999</v>
       </c>
-      <c r="L10" s="27">
+      <c r="L10" s="29">
         <v>0.79890000000000005</v>
       </c>
-      <c r="M10" s="27">
+      <c r="M10" s="29">
         <v>0.87380000000000002</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="26" customFormat="1" ht="30" customHeight="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="20" customFormat="1" ht="30" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2">
         <v>224</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11" s="4">
         <v>0.94850000000000001</v>
@@ -1891,33 +1931,33 @@
         <v>0.83840000000000003</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2">
         <v>224</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I12" s="4">
         <v>0.92720000000000002</v>
@@ -1935,33 +1975,33 @@
         <v>0.85860000000000003</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2">
         <v>224</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13" s="4">
         <v>0.92600000000000005</v>
@@ -1979,33 +2019,33 @@
         <v>0.84909999999999997</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="30" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2">
         <v>224</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14" s="4">
         <v>0.88039999999999996</v>
@@ -2023,246 +2063,338 @@
         <v>0.87770000000000004</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="30" customHeight="1">
-      <c r="A15" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="20" customFormat="1" ht="30" customHeight="1">
+      <c r="A15" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="2">
+        <v>224</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0.81289999999999996</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0.76880000000000004</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0.79979999999999996</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0.87070000000000003</v>
+      </c>
+      <c r="N15" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="17">
-        <v>224</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="15">
-        <v>0.89300000000000002</v>
-      </c>
-      <c r="J15" s="15">
-        <v>0.81289999999999996</v>
-      </c>
-      <c r="K15" s="15">
-        <v>0.76880000000000004</v>
-      </c>
-      <c r="L15" s="15">
-        <v>0.79979999999999996</v>
-      </c>
-      <c r="M15" s="15">
-        <v>0.87070000000000003</v>
-      </c>
-      <c r="N15" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" s="26" customFormat="1" ht="30" customHeight="1">
+    </row>
+    <row r="16" spans="1:14" s="20" customFormat="1" ht="30" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2">
         <v>320</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0.88959999999999995</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.82150000000000001</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0.7762</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0.80630000000000002</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0.88129999999999997</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="17" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="22">
+      <c r="A17" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="17">
+        <v>320</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="15">
+        <v>0.91769999999999996</v>
+      </c>
+      <c r="J17" s="15">
+        <v>0.80120000000000002</v>
+      </c>
+      <c r="K17" s="15">
+        <v>0.7742</v>
+      </c>
+      <c r="L17" s="15">
+        <v>0.75729999999999997</v>
+      </c>
+      <c r="M17" s="15">
+        <v>0.86370000000000002</v>
+      </c>
+      <c r="N17" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="17">
+        <v>320</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="15">
+        <v>0.91139999999999999</v>
+      </c>
+      <c r="J18" s="15">
+        <v>0.82820000000000005</v>
+      </c>
+      <c r="K18" s="15">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="L18" s="15">
+        <v>0.78639999999999999</v>
+      </c>
+      <c r="M18" s="15">
+        <v>0.89629999999999999</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="18" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+    </row>
+    <row r="20" spans="1:14" s="20" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="23">
         <v>224</v>
       </c>
-      <c r="D17" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="I17" s="24">
+      <c r="D20" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="25">
         <v>0.96609999999999996</v>
       </c>
-      <c r="J17" s="24">
+      <c r="J20" s="25">
         <v>0.86040000000000005</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K20" s="21">
         <v>0.83279999999999998</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L20" s="21">
         <v>0.85829999999999995</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M20" s="21">
         <v>0.89549999999999996</v>
       </c>
-      <c r="N17" s="25" t="s">
+      <c r="N20" s="21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="20" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="23">
+        <v>224</v>
+      </c>
+      <c r="D21" s="24" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" s="26" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="33">
-        <v>224</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="H18" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="I18" s="35">
+      <c r="E21" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" s="25">
         <v>0.96519999999999995</v>
       </c>
-      <c r="J18" s="35">
+      <c r="J21" s="25">
         <v>0.84470000000000001</v>
       </c>
-      <c r="K18" s="28">
+      <c r="K21" s="21">
         <v>0.81889999999999996</v>
       </c>
-      <c r="L18" s="28">
+      <c r="L21" s="21">
         <v>0.83930000000000005</v>
       </c>
-      <c r="M18" s="28">
+      <c r="M21" s="21">
         <v>0.88109999999999999</v>
       </c>
-      <c r="N18" s="28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="30" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-    </row>
-    <row r="20" spans="1:14" ht="30" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-    </row>
-    <row r="21" spans="1:14" ht="30" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-    </row>
-    <row r="22" spans="1:14" ht="30" customHeight="1">
-      <c r="A22" s="7"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
+      <c r="N21" s="21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="35" customFormat="1" ht="30" customHeight="1">
+      <c r="A22" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="32">
+        <v>320</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="34">
+        <v>0.96809999999999996</v>
+      </c>
+      <c r="J22" s="34">
+        <v>0.88370000000000004</v>
+      </c>
+      <c r="K22" s="34">
+        <v>0.86060000000000003</v>
+      </c>
+      <c r="L22" s="34">
+        <v>0.85650000000000004</v>
+      </c>
+      <c r="M22" s="34">
+        <v>0.92849999999999999</v>
+      </c>
+      <c r="N22" s="30" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="23" spans="1:14" ht="30" customHeight="1">
       <c r="A23" s="7"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -2273,6 +2405,56 @@
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="1:14" ht="30" customHeight="1">
+      <c r="A24" s="7"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" spans="1:14" ht="30" customHeight="1">
+      <c r="A25" s="7"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+    </row>
+    <row r="26" spans="1:14" ht="30" customHeight="1">
+      <c r="A26" s="7"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2295,808 +2477,808 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="20" t="s">
-        <v>42</v>
+      <c r="A1" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B1">
         <v>0.77490000000000003</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="20" t="s">
-        <v>42</v>
+      <c r="A2" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B2">
         <v>0.77690000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="20" t="s">
-        <v>42</v>
+      <c r="A3" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B3">
         <v>0.77739999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="20" t="s">
-        <v>42</v>
+      <c r="A4" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B4">
         <v>0.77949999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="20" t="s">
-        <v>42</v>
+      <c r="A5" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B5">
         <v>0.78049999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="20" t="s">
-        <v>42</v>
+      <c r="A6" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B6">
         <v>0.78100000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="20" t="s">
-        <v>42</v>
+      <c r="A7" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B7">
         <v>0.78249999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="20" t="s">
-        <v>42</v>
+      <c r="A8" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B8">
         <v>0.78400000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="20" t="s">
-        <v>42</v>
+      <c r="A9" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B9">
         <v>0.78400000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="20" t="s">
-        <v>42</v>
+      <c r="A10" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B10">
         <v>0.78549999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="20" t="s">
-        <v>42</v>
+      <c r="A11" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B11">
         <v>0.78710000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="20" t="s">
-        <v>42</v>
+      <c r="A12" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B12">
         <v>0.78759999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="20" t="s">
-        <v>42</v>
+      <c r="A13" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B13">
         <v>0.78859999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="20" t="s">
-        <v>42</v>
+      <c r="A14" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B14">
         <v>0.78910000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="20" t="s">
-        <v>42</v>
+      <c r="A15" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B15">
         <v>0.79059999999999997</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="20" t="s">
-        <v>42</v>
+      <c r="A16" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B16">
         <v>0.79410000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="20" t="s">
-        <v>42</v>
+      <c r="A17" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B17">
         <v>0.79510000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="20" t="s">
-        <v>42</v>
+      <c r="A18" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B18">
         <v>0.79669999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="20" t="s">
-        <v>42</v>
+      <c r="A19" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B19">
         <v>0.79920000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="20" t="s">
-        <v>42</v>
+      <c r="A20" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B20">
         <v>0.79969999999999997</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="20" t="s">
-        <v>42</v>
+      <c r="A21" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B21">
         <v>0.80069999999999997</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="20" t="s">
-        <v>42</v>
+      <c r="A22" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B22">
         <v>0.80069999999999997</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="20" t="s">
-        <v>42</v>
+      <c r="A23" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B23">
         <v>0.80220000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="20" t="s">
-        <v>42</v>
+      <c r="A24" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B24">
         <v>0.80420000000000003</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="20" t="s">
-        <v>42</v>
+      <c r="A25" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B25">
         <v>0.80579999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="20" t="s">
-        <v>42</v>
+      <c r="A26" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B26">
         <v>0.80679999999999996</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="20" t="s">
-        <v>42</v>
+      <c r="A27" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B27">
         <v>0.80779999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="20" t="s">
-        <v>42</v>
+      <c r="A28" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B28">
         <v>0.80879999999999996</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="20" t="s">
-        <v>42</v>
+      <c r="A29" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B29">
         <v>0.81340000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="20" t="s">
-        <v>42</v>
+      <c r="A30" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B30">
         <v>0.81440000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="20" t="s">
-        <v>42</v>
+      <c r="A31" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B31">
         <v>0.81340000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="20" t="s">
-        <v>42</v>
+      <c r="A32" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B32">
         <v>0.81489999999999996</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="20" t="s">
-        <v>42</v>
+      <c r="A33" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B33">
         <v>0.81540000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="20" t="s">
-        <v>42</v>
+      <c r="A34" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B34">
         <v>0.81840000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="20" t="s">
-        <v>42</v>
+      <c r="A35" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B35">
         <v>0.82199999999999995</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="20" t="s">
-        <v>42</v>
+      <c r="A36" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B36">
         <v>0.82250000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="20" t="s">
-        <v>42</v>
+      <c r="A37" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B37">
         <v>0.82350000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="20" t="s">
-        <v>42</v>
+      <c r="A38" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B38">
         <v>0.82550000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="20" t="s">
-        <v>42</v>
+      <c r="A39" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B39">
         <v>0.82799999999999996</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="20" t="s">
-        <v>42</v>
+      <c r="A40" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B40">
         <v>0.83509999999999995</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="20" t="s">
-        <v>42</v>
+      <c r="A41" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B41">
         <v>0.83609999999999995</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="20" t="s">
-        <v>42</v>
+      <c r="A42" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B42">
         <v>0.83809999999999996</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="20" t="s">
-        <v>42</v>
+      <c r="A43" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B43">
         <v>0.83709999999999996</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="20" t="s">
-        <v>42</v>
+      <c r="A44" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B44">
         <v>0.83809999999999996</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="20" t="s">
-        <v>42</v>
+      <c r="A45" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B45">
         <v>0.8407</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="20" t="s">
-        <v>42</v>
+      <c r="A46" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B46">
         <v>0.84319999999999995</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="20" t="s">
-        <v>42</v>
+      <c r="A47" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B47">
         <v>0.84219999999999995</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="20" t="s">
-        <v>42</v>
+      <c r="A48" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B48">
         <v>0.84470000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="20" t="s">
-        <v>42</v>
+      <c r="A49" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B49">
         <v>0.84770000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="20" t="s">
-        <v>42</v>
+      <c r="A50" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B50">
         <v>0.8488</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="20" t="s">
-        <v>42</v>
+      <c r="A51" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B51">
         <v>0.84470000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="20" t="s">
-        <v>42</v>
+      <c r="A52" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B52">
         <v>0.84719999999999995</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="20" t="s">
-        <v>42</v>
+      <c r="A53" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B53">
         <v>0.8498</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="20" t="s">
-        <v>42</v>
+      <c r="A54" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B54">
         <v>0.85129999999999995</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="20" t="s">
-        <v>42</v>
+      <c r="A55" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B55">
         <v>0.8508</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="20" t="s">
-        <v>42</v>
+      <c r="A56" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B56">
         <v>0.84830000000000005</v>
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="20" t="s">
-        <v>42</v>
+      <c r="A57" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B57">
         <v>0.84719999999999995</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="20" t="s">
-        <v>42</v>
+      <c r="A58" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B58">
         <v>0.84570000000000001</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="20" t="s">
-        <v>42</v>
+      <c r="A59" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B59">
         <v>0.84319999999999995</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="20" t="s">
-        <v>42</v>
+      <c r="A60" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B60">
         <v>0.84219999999999995</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="20" t="s">
-        <v>42</v>
+      <c r="A61" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B61">
         <v>0.83709999999999996</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="20" t="s">
-        <v>42</v>
+      <c r="A62" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B62">
         <v>0.83509999999999995</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="20" t="s">
-        <v>42</v>
+      <c r="A63" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B63">
         <v>0.83409999999999995</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="20" t="s">
-        <v>42</v>
+      <c r="A64" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B64">
         <v>0.8306</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="20" t="s">
-        <v>42</v>
+      <c r="A65" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B65">
         <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="20" t="s">
-        <v>42</v>
+      <c r="A66" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B66">
         <v>0.82550000000000001</v>
       </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="20" t="s">
-        <v>42</v>
+      <c r="A67" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B67">
         <v>0.82350000000000001</v>
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="20" t="s">
-        <v>42</v>
+      <c r="A68" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B68">
         <v>0.82140000000000002</v>
       </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="20" t="s">
-        <v>42</v>
+      <c r="A69" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B69">
         <v>0.81940000000000002</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="20" t="s">
-        <v>42</v>
+      <c r="A70" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B70">
         <v>0.81840000000000002</v>
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="20" t="s">
-        <v>42</v>
+      <c r="A71" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B71">
         <v>0.81689999999999996</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="20" t="s">
-        <v>42</v>
+      <c r="A72" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B72">
         <v>0.81589999999999996</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="20" t="s">
-        <v>42</v>
+      <c r="A73" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B73">
         <v>0.81440000000000001</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="20" t="s">
-        <v>42</v>
+      <c r="A74" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B74">
         <v>0.81340000000000001</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="20" t="s">
-        <v>42</v>
+      <c r="A75" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B75">
         <v>0.81279999999999997</v>
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="20" t="s">
-        <v>42</v>
+      <c r="A76" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B76">
         <v>0.81279999999999997</v>
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="20" t="s">
-        <v>42</v>
+      <c r="A77" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B77">
         <v>0.81279999999999997</v>
       </c>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" s="20" t="s">
-        <v>42</v>
+      <c r="A78" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B78">
         <v>0.81340000000000001</v>
       </c>
     </row>
     <row r="79" spans="1:2">
-      <c r="A79" s="20" t="s">
-        <v>42</v>
+      <c r="A79" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B79">
         <v>0.81130000000000002</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="20" t="s">
-        <v>42</v>
+      <c r="A80" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B80">
         <v>0.81130000000000002</v>
       </c>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="20" t="s">
-        <v>42</v>
+      <c r="A81" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B81">
         <v>0.81130000000000002</v>
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="20" t="s">
-        <v>42</v>
+      <c r="A82" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B82">
         <v>0.80979999999999996</v>
       </c>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="20" t="s">
-        <v>42</v>
+      <c r="A83" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B83">
         <v>0.80879999999999996</v>
       </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="20" t="s">
-        <v>42</v>
+      <c r="A84" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B84">
         <v>0.80979999999999996</v>
       </c>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="20" t="s">
-        <v>42</v>
+      <c r="A85" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B85">
         <v>0.80930000000000002</v>
       </c>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="20" t="s">
-        <v>42</v>
+      <c r="A86" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B86">
         <v>0.80879999999999996</v>
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="20" t="s">
-        <v>42</v>
+      <c r="A87" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B87">
         <v>0.81030000000000002</v>
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="20" t="s">
-        <v>42</v>
+      <c r="A88" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B88">
         <v>0.81030000000000002</v>
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="20" t="s">
-        <v>42</v>
+      <c r="A89" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B89">
         <v>0.80930000000000002</v>
       </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="20" t="s">
-        <v>42</v>
+      <c r="A90" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B90">
         <v>0.80879999999999996</v>
       </c>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" s="20" t="s">
-        <v>42</v>
+      <c r="A91" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B91">
         <v>0.80779999999999996</v>
       </c>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" s="20" t="s">
-        <v>42</v>
+      <c r="A92" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B92">
         <v>0.80730000000000002</v>
       </c>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" s="20" t="s">
-        <v>42</v>
+      <c r="A93" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B93">
         <v>0.80479999999999996</v>
       </c>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="20" t="s">
-        <v>42</v>
+      <c r="A94" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B94">
         <v>0.80269999999999997</v>
       </c>
     </row>
     <row r="95" spans="1:2">
-      <c r="A95" s="20" t="s">
-        <v>42</v>
+      <c r="A95" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B95">
         <v>0.80220000000000002</v>
       </c>
     </row>
     <row r="96" spans="1:2">
-      <c r="A96" s="20" t="s">
-        <v>42</v>
+      <c r="A96" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B96">
         <v>0.80269999999999997</v>
       </c>
     </row>
     <row r="97" spans="1:2">
-      <c r="A97" s="20" t="s">
-        <v>42</v>
+      <c r="A97" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B97">
         <v>0.80220000000000002</v>
       </c>
     </row>
     <row r="98" spans="1:2">
-      <c r="A98" s="20" t="s">
-        <v>42</v>
+      <c r="A98" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B98">
         <v>0.80069999999999997</v>
       </c>
     </row>
     <row r="99" spans="1:2">
-      <c r="A99" s="20" t="s">
-        <v>42</v>
+      <c r="A99" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B99">
         <v>0.79920000000000002</v>
       </c>
     </row>
     <row r="100" spans="1:2">
-      <c r="A100" s="20" t="s">
-        <v>42</v>
+      <c r="A100" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B100">
         <v>0.79869999999999997</v>
       </c>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="20" t="s">
-        <v>42</v>
+      <c r="A101" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B101">
         <v>0.79820000000000002</v>
@@ -3114,201 +3296,209 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="2" max="2" width="8.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1">
-        <v>0.80020000000000002</v>
+        <v>0.82850000000000001</v>
       </c>
       <c r="C1">
         <f>B1+B6+B11+B16+B21</f>
-        <v>4.0647000000000002</v>
+        <v>4.1411999999999995</v>
       </c>
       <c r="D1">
         <f>C1/5</f>
-        <v>0.81294</v>
+        <v>0.82823999999999987</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2">
-        <v>0.76249999999999996</v>
+        <v>0.79210000000000003</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C4" si="0">B2+B7+B12+B17+B22</f>
-        <v>3.8441999999999998</v>
+        <v>3.9569000000000001</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D4" si="1">C2/5</f>
-        <v>0.76883999999999997</v>
+        <v>0.79137999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3">
-        <v>0.76519999999999999</v>
+        <v>0.78259999999999996</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
-        <v>3.9990999999999999</v>
+        <v>3.9318999999999997</v>
       </c>
       <c r="D3">
         <f t="shared" si="1"/>
-        <v>0.79981999999999998</v>
+        <v>0.78637999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4">
-        <v>0.86619999999999997</v>
+        <v>0.89829999999999999</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>4.3533999999999997</v>
+        <v>4.4813999999999998</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>0.8706799999999999</v>
+        <v>0.89627999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
-        <v>0.81079999999999997</v>
+        <v>0.82199999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7">
-        <v>0.76429999999999998</v>
+        <v>0.7863</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8">
-        <v>0.80210000000000004</v>
+        <v>0.77170000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9">
-        <v>0.86939999999999995</v>
+        <v>0.89419999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11">
-        <v>0.80420000000000003</v>
+        <v>0.82799999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12">
-        <v>0.76600000000000001</v>
+        <v>0.79139999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13">
-        <v>0.78</v>
+        <v>0.78990000000000005</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14">
-        <v>0.86439999999999995</v>
+        <v>0.89400000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16">
-        <v>0.82750000000000001</v>
+        <v>0.83209999999999995</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17">
-        <v>0.78139999999999998</v>
+        <v>0.79430000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18">
-        <v>0.82520000000000004</v>
+        <v>0.7974</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19">
-        <v>0.87880000000000003</v>
+        <v>0.89659999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21">
-        <v>0.82199999999999995</v>
+        <v>0.8306</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22">
-        <v>0.77</v>
+        <v>0.79279999999999995</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23">
-        <v>0.8266</v>
+        <v>0.7903</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24">
-        <v>0.87460000000000004</v>
+        <v>0.89829999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>